<commit_message>
ngmiho add folder image/readme
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/report.xlsx
+++ b/src/main/webapp/report/report.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2024 2 292024 2 29" r:id="rId3" sheetId="1"/>
+    <sheet name="2024 1 1" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -17,7 +17,7 @@
     <t>#</t>
   </si>
   <si>
-    <t>Drink Name</t>
+    <t>Create Date</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -26,7 +26,7 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>The Coffee House Sữa Đá</t>
+    <t>2024-01-01T00:00</t>
   </si>
 </sst>
 </file>
@@ -99,10 +99,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D2" t="n">
-        <v>39000.0</v>
+        <v>65000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>